<commit_message>
Properly animate clustered species
Finally worked out the right way to plot things. Want to look into dbscan method more though to implement clustering - seems more like what Ryan was describing
</commit_message>
<xml_diff>
--- a/headings.xlsx
+++ b/headings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Kmax</t>
   </si>
@@ -84,6 +84,69 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>bottom temp</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>year, sample #, month</t>
+  </si>
+  <si>
+    <t>unique id for space &amp; time of haul</t>
+  </si>
+  <si>
+    <t>weight catch per unit effort - measure of biomass</t>
+  </si>
+  <si>
+    <t>effort: area of sf sampled</t>
+  </si>
+  <si>
+    <t>catch: kg</t>
+  </si>
+  <si>
+    <t>kg/area</t>
+  </si>
+  <si>
+    <t>surface temp</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>region identifier - ebs</t>
+  </si>
+  <si>
+    <t>combination of long lat depth</t>
+  </si>
+  <si>
+    <t>same as spp</t>
+  </si>
+  <si>
+    <t>1 in most cases</t>
+  </si>
+  <si>
+    <t>number of samples per place &amp; time</t>
+  </si>
+  <si>
+    <t># of indiv</t>
+  </si>
+  <si>
+    <t>don't read into</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>number of hauls w/in stratum year combo</t>
+  </si>
+  <si>
+    <t>indicator of replicates in stratum year</t>
+  </si>
+  <si>
+    <t>1 to 4</t>
   </si>
 </sst>
 </file>
@@ -119,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,13 +499,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="27.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -503,6 +579,83 @@
       </c>
       <c r="T1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>